<commit_message>
Updates everything with new assignspecies tables; NEARLY COMPLETE; (all tables updates
</commit_message>
<xml_diff>
--- a/Deliverables/Copy of WADE003-arcticpred-16SP2-taxa-mapped_1.xlsx
+++ b/Deliverables/Copy of WADE003-arcticpred-16SP2-taxa-mapped_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{691F6B23-B4D5-4FBA-8A11-FE9B762346EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D3CC3BB-1312-4A71-9470-50EBA9AA2E05}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{691F6B23-B4D5-4FBA-8A11-FE9B762346EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B489E8CB-CA30-4F5C-8098-874E4FA3378B}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-24000" yWindow="1230" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mapped" sheetId="1" r:id="rId1"/>
@@ -2065,7 +2065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
@@ -3877,7 +3877,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3889,8 +3889,8 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="96" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.42578125" customWidth="1"/>
+    <col min="10" max="10" width="109.42578125" customWidth="1"/>
     <col min="11" max="11" width="255.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4415,7 +4415,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4427,7 +4427,7 @@
     <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="109.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="255.5703125" style="3" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>